<commit_message>
primer commit en branc prueba uno
</commit_message>
<xml_diff>
--- a/NOMINA EMISION GRUPAL.xlsx
+++ b/NOMINA EMISION GRUPAL.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laura\Desktop\AGENCIA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\LollaPalluza-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CB92991-BC6E-47D2-B1CE-5B293B716157}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73349186-19C8-4446-9183-9C6B00444033}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Nómina de Pasajeros</t>
   </si>
@@ -94,12 +93,18 @@
   </si>
   <si>
     <t>PNR RESERVADO</t>
+  </si>
+  <si>
+    <t>hola Laura</t>
+  </si>
+  <si>
+    <t>:)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
@@ -377,9 +382,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -420,28 +422,31 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{CF4B7E01-4879-4343-936F-335404213636}"/>
+    <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Sheet1" xfId="2" xr:uid="{B067EE63-6562-4AA6-816F-188FC1267F7C}"/>
+    <cellStyle name="Normal_Sheet1" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -752,11 +757,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D09E9671-04E0-45FE-AB20-5F7441BC49B6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,529 +781,533 @@
       <c r="B1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="23" t="s">
+      <c r="K3" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="23" t="s">
+      <c r="L3" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="24" t="s">
+      <c r="M3" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="24" t="s">
+      <c r="N3" s="22" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="11">
+      <c r="A4" s="3"/>
+      <c r="B4" s="10">
         <v>1</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="11">
+      <c r="C4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="13"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="10">
         <v>1</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="11">
+      <c r="A5" s="3"/>
+      <c r="B5" s="10">
         <v>2</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="11">
+      <c r="C5" s="15"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="10">
         <v>2</v>
       </c>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="11">
+      <c r="A6" s="3"/>
+      <c r="B6" s="10">
         <v>3</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="11">
+      <c r="C6" s="15"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="10">
         <v>3</v>
       </c>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="11">
+      <c r="A7" s="3"/>
+      <c r="B7" s="10">
         <v>4</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="11">
+      <c r="C7" s="15"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="10">
         <v>4</v>
       </c>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="11">
+      <c r="A8" s="3"/>
+      <c r="B8" s="10">
         <v>5</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="11">
+      <c r="C8" s="15"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="10">
         <v>5</v>
       </c>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="11">
+      <c r="A9" s="3"/>
+      <c r="B9" s="10">
         <v>6</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="11">
+      <c r="C9" s="15"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="10">
         <v>6</v>
       </c>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="11">
+      <c r="A10" s="3"/>
+      <c r="B10" s="10">
         <v>7</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="11">
+      <c r="C10" s="15"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="10">
         <v>7</v>
       </c>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="11">
+      <c r="A11" s="3"/>
+      <c r="B11" s="10">
         <v>8</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="11">
+      <c r="C11" s="15"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="10">
         <v>8</v>
       </c>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="11">
+      <c r="A12" s="3"/>
+      <c r="B12" s="10">
         <v>9</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="11">
+      <c r="C12" s="15"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="10">
         <v>9</v>
       </c>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="11">
+      <c r="A13" s="3"/>
+      <c r="B13" s="10">
         <v>10</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="11">
+      <c r="C13" s="15"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="10">
         <v>10</v>
       </c>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="25"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="11">
+      <c r="A14" s="3"/>
+      <c r="B14" s="10">
         <v>11</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="11">
+      <c r="C14" s="15"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="10">
         <v>11</v>
       </c>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="11">
+      <c r="A15" s="3"/>
+      <c r="B15" s="10">
         <v>12</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="11">
+      <c r="C15" s="15"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="10">
         <v>12</v>
       </c>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="25"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="11">
+      <c r="A16" s="3"/>
+      <c r="B16" s="10">
         <v>13</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="11">
+      <c r="C16" s="15"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="10">
         <v>13</v>
       </c>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="25"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="11">
+      <c r="A17" s="3"/>
+      <c r="B17" s="10">
         <v>14</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="11">
+      <c r="C17" s="15"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="10">
         <v>14</v>
       </c>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="11">
+      <c r="A18" s="3"/>
+      <c r="B18" s="10">
         <v>15</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="11">
+      <c r="C18" s="15"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="10">
         <v>15</v>
       </c>
-      <c r="H18" s="25"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="25"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="11">
+      <c r="A19" s="3"/>
+      <c r="B19" s="10">
         <v>16</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="11">
+      <c r="C19" s="15"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="10">
         <v>16</v>
       </c>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="25"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="11">
+      <c r="A20" s="3"/>
+      <c r="B20" s="10">
         <v>17</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="11">
+      <c r="C20" s="15"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="10">
         <v>17</v>
       </c>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="25"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="25"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="11">
+      <c r="A21" s="3"/>
+      <c r="B21" s="10">
         <v>18</v>
       </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="11">
+      <c r="C21" s="15"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="10">
         <v>18</v>
       </c>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="25"/>
-      <c r="N21" s="25"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="11">
+      <c r="A22" s="3"/>
+      <c r="B22" s="10">
         <v>19</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="11">
+      <c r="C22" s="15"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="10">
         <v>19</v>
       </c>
-      <c r="H22" s="25"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="25"/>
-      <c r="N22" s="25"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="11">
+      <c r="A23" s="3"/>
+      <c r="B23" s="10">
         <v>20</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="11">
+      <c r="C23" s="15"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="10">
         <v>20</v>
       </c>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="25"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="11">
+      <c r="A24" s="3"/>
+      <c r="B24" s="10">
         <v>21</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="11">
+      <c r="C24" s="15"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="10">
         <v>21</v>
       </c>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
-      <c r="M24" s="25"/>
-      <c r="N24" s="25"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="11">
+      <c r="A25" s="3"/>
+      <c r="B25" s="10">
         <v>22</v>
       </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="11">
+      <c r="C25" s="15"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="10">
         <v>22</v>
       </c>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="25"/>
-      <c r="N25" s="25"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
     </row>
     <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19"/>
-      <c r="M26" s="19"/>
-      <c r="N26" s="25"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="23"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
@@ -1314,7 +1323,7 @@
       <c r="C29" t="s">
         <v>16</v>
       </c>
-      <c r="K29" s="26"/>
+      <c r="K29" s="24"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C30" t="s">

</xml_diff>